<commit_message>
fixing national + other stuff
</commit_message>
<xml_diff>
--- a/national_dta.xlsx
+++ b/national_dta.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19380" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Education" sheetId="3" r:id="rId1"/>
@@ -526,7 +526,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
@@ -2064,14 +2064,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D66"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="80.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -2082,10 +2083,10 @@
         <v>8</v>
       </c>
       <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
         <v>9</v>
-      </c>
-      <c r="D1" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2096,10 +2097,10 @@
         <v>5</v>
       </c>
       <c r="C2">
-        <v>282005382</v>
+        <v>316515008</v>
       </c>
       <c r="D2">
-        <v>316515021</v>
+        <v>222464704</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -2110,10 +2111,10 @@
         <v>45</v>
       </c>
       <c r="C3">
-        <v>22958219</v>
+        <v>16235305</v>
       </c>
       <c r="D3">
-        <v>16235305</v>
+        <v>8769653</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -2124,10 +2125,10 @@
         <v>15</v>
       </c>
       <c r="C4">
-        <v>4716473</v>
+        <v>3303512</v>
       </c>
       <c r="D4">
-        <v>3303512</v>
+        <v>1434568</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -2138,10 +2139,10 @@
         <v>16</v>
       </c>
       <c r="C5">
-        <v>210351</v>
+        <v>153234</v>
       </c>
       <c r="D5">
-        <v>153234</v>
+        <v>64614</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -2152,10 +2153,10 @@
         <v>17</v>
       </c>
       <c r="C6">
-        <v>350950</v>
+        <v>263396</v>
       </c>
       <c r="D6">
-        <v>263396</v>
+        <v>158556</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -2166,10 +2167,10 @@
         <v>6</v>
       </c>
       <c r="C7">
-        <v>5414353</v>
+        <v>3852099</v>
       </c>
       <c r="D7">
-        <v>3693977</v>
+        <v>2087394</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -2180,10 +2181,10 @@
         <v>18</v>
       </c>
       <c r="C8">
-        <v>229618</v>
+        <v>148275</v>
       </c>
       <c r="D8">
-        <v>148275</v>
+        <v>94681</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -2194,10 +2195,10 @@
         <v>19</v>
       </c>
       <c r="C9">
-        <v>3931110</v>
+        <v>2717844</v>
       </c>
       <c r="D9">
-        <v>2717844</v>
+        <v>1713835</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -2208,10 +2209,10 @@
         <v>20</v>
       </c>
       <c r="C10">
-        <v>262119</v>
+        <v>267009</v>
       </c>
       <c r="D10">
-        <v>267009</v>
+        <v>140899</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -2222,10 +2223,10 @@
         <v>21</v>
       </c>
       <c r="C11">
-        <v>108823</v>
+        <v>71451</v>
       </c>
       <c r="D11">
-        <v>71451</v>
+        <v>24703</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -2236,10 +2237,10 @@
         <v>22</v>
       </c>
       <c r="C12">
-        <v>993935</v>
+        <v>779637</v>
       </c>
       <c r="D12">
-        <v>779637</v>
+        <v>500155</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -2250,10 +2251,10 @@
         <v>23</v>
       </c>
       <c r="C13">
-        <v>2191253</v>
+        <v>1460214</v>
       </c>
       <c r="D13">
-        <v>1460214</v>
+        <v>810630</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -2264,10 +2265,10 @@
         <v>24</v>
       </c>
       <c r="C14">
-        <v>278479</v>
+        <v>207999</v>
       </c>
       <c r="D14">
-        <v>207999</v>
+        <v>124308</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -2278,10 +2279,10 @@
         <v>25</v>
       </c>
       <c r="C15">
-        <v>31391</v>
+        <v>18803</v>
       </c>
       <c r="D15">
-        <v>18803</v>
+        <v>5648</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -2292,10 +2293,10 @@
         <v>26</v>
       </c>
       <c r="C16">
-        <v>546088</v>
+        <v>414880</v>
       </c>
       <c r="D16">
-        <v>414880</v>
+        <v>204726</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -2306,10 +2307,10 @@
         <v>27</v>
       </c>
       <c r="C17">
-        <v>69880</v>
+        <v>46036</v>
       </c>
       <c r="D17">
-        <v>46036</v>
+        <v>20164</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -2320,10 +2321,10 @@
         <v>28</v>
       </c>
       <c r="C18">
-        <v>298681</v>
+        <v>188673</v>
       </c>
       <c r="D18">
-        <v>188673</v>
+        <v>104884</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -2334,10 +2335,10 @@
         <v>29</v>
       </c>
       <c r="C19">
-        <v>2430258</v>
+        <v>1710547</v>
       </c>
       <c r="D19">
-        <v>1710547</v>
+        <v>1065739</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -2348,10 +2349,10 @@
         <v>46</v>
       </c>
       <c r="C20">
-        <v>24908927</v>
+        <v>19167716</v>
       </c>
       <c r="D20">
-        <v>19167716</v>
+        <v>10138697</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -2362,10 +2363,10 @@
         <v>15</v>
       </c>
       <c r="C21">
-        <v>4963074</v>
+        <v>3590279</v>
       </c>
       <c r="D21">
-        <v>3590279</v>
+        <v>1558594</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -2376,10 +2377,10 @@
         <v>16</v>
       </c>
       <c r="C22">
-        <v>223625</v>
+        <v>164821</v>
       </c>
       <c r="D22">
-        <v>164821</v>
+        <v>69825</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -2390,10 +2391,10 @@
         <v>17</v>
       </c>
       <c r="C23">
-        <v>382247</v>
+        <v>316640</v>
       </c>
       <c r="D23">
-        <v>316640</v>
+        <v>176113</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -2404,10 +2405,10 @@
         <v>6</v>
       </c>
       <c r="C24">
-        <v>5925834</v>
+        <v>4597905</v>
       </c>
       <c r="D24">
-        <v>4428363</v>
+        <v>2459584</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -2418,10 +2419,10 @@
         <v>18</v>
       </c>
       <c r="C25">
-        <v>256911</v>
+        <v>181029</v>
       </c>
       <c r="D25">
-        <v>181029</v>
+        <v>109715</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -2432,10 +2433,10 @@
         <v>19</v>
       </c>
       <c r="C26">
-        <v>4504514</v>
+        <v>3707082</v>
       </c>
       <c r="D26">
-        <v>3707082</v>
+        <v>2181775</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -2446,10 +2447,10 @@
         <v>20</v>
       </c>
       <c r="C27">
-        <v>269245</v>
+        <v>280410</v>
       </c>
       <c r="D27">
-        <v>280410</v>
+        <v>144882</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -2460,10 +2461,10 @@
         <v>21</v>
       </c>
       <c r="C28">
-        <v>140602</v>
+        <v>108477</v>
       </c>
       <c r="D28">
-        <v>108477</v>
+        <v>41617</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -2474,10 +2475,10 @@
         <v>22</v>
       </c>
       <c r="C29">
-        <v>1361511</v>
+        <v>1388163</v>
       </c>
       <c r="D29">
-        <v>1388163</v>
+        <v>831898</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -2488,10 +2489,10 @@
         <v>23</v>
       </c>
       <c r="C30">
-        <v>2355511</v>
+        <v>1792437</v>
       </c>
       <c r="D30">
-        <v>1792437</v>
+        <v>953489</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
@@ -2502,10 +2503,10 @@
         <v>24</v>
       </c>
       <c r="C31">
-        <v>299409</v>
+        <v>256416</v>
       </c>
       <c r="D31">
-        <v>256416</v>
+        <v>137527</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -2516,10 +2517,10 @@
         <v>25</v>
       </c>
       <c r="C32">
-        <v>42197</v>
+        <v>28818</v>
       </c>
       <c r="D32">
-        <v>28818</v>
+        <v>9973</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
@@ -2530,10 +2531,10 @@
         <v>26</v>
       </c>
       <c r="C33">
-        <v>578493</v>
+        <v>455005</v>
       </c>
       <c r="D33">
-        <v>455005</v>
+        <v>222252</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
@@ -2544,10 +2545,10 @@
         <v>27</v>
       </c>
       <c r="C34">
-        <v>74505</v>
+        <v>52267</v>
       </c>
       <c r="D34">
-        <v>52267</v>
+        <v>22161</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -2558,10 +2559,10 @@
         <v>28</v>
       </c>
       <c r="C35">
-        <v>348110</v>
+        <v>278281</v>
       </c>
       <c r="D35">
-        <v>278281</v>
+        <v>142232</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
@@ -2572,10 +2573,10 @@
         <v>29</v>
       </c>
       <c r="C36">
-        <v>2583533</v>
+        <v>1928363</v>
       </c>
       <c r="D36">
-        <v>1928363</v>
+        <v>1163357</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
@@ -2586,10 +2587,10 @@
         <v>47</v>
       </c>
       <c r="C37">
-        <v>500510</v>
+        <v>546255</v>
       </c>
       <c r="D37">
-        <v>546255</v>
+        <v>332580</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
@@ -2600,10 +2601,10 @@
         <v>30</v>
       </c>
       <c r="C38">
-        <v>288500</v>
+        <v>1262434</v>
       </c>
       <c r="D38">
-        <v>344487</v>
+        <v>748301</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
@@ -2613,12 +2614,6 @@
       <c r="B39" t="s">
         <v>31</v>
       </c>
-      <c r="C39">
-        <v>138775</v>
-      </c>
-      <c r="D39">
-        <v>174460</v>
-      </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
@@ -2627,12 +2622,6 @@
       <c r="B40" t="s">
         <v>32</v>
       </c>
-      <c r="C40">
-        <v>90498</v>
-      </c>
-      <c r="D40">
-        <v>109455</v>
-      </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
@@ -2641,12 +2630,6 @@
       <c r="B41" t="s">
         <v>33</v>
       </c>
-      <c r="C41">
-        <v>48207</v>
-      </c>
-      <c r="D41">
-        <v>45453</v>
-      </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
@@ -2655,12 +2638,6 @@
       <c r="B42" t="s">
         <v>34</v>
       </c>
-      <c r="C42">
-        <v>134080</v>
-      </c>
-      <c r="D42">
-        <v>138360</v>
-      </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
@@ -2669,12 +2646,6 @@
       <c r="B43" t="s">
         <v>35</v>
       </c>
-      <c r="C43">
-        <v>60527</v>
-      </c>
-      <c r="D43">
-        <v>73088</v>
-      </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
@@ -2683,12 +2654,6 @@
       <c r="B44" t="s">
         <v>36</v>
       </c>
-      <c r="C44">
-        <v>49263</v>
-      </c>
-      <c r="D44">
-        <v>34239</v>
-      </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
@@ -2697,12 +2662,6 @@
       <c r="B45" t="s">
         <v>37</v>
       </c>
-      <c r="C45">
-        <v>48239</v>
-      </c>
-      <c r="D45">
-        <v>33468</v>
-      </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
@@ -2711,12 +2670,6 @@
       <c r="B46" t="s">
         <v>48</v>
       </c>
-      <c r="C46">
-        <v>1037116</v>
-      </c>
-      <c r="D46">
-        <v>1262434</v>
-      </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
@@ -2725,12 +2678,6 @@
       <c r="B47" t="s">
         <v>30</v>
       </c>
-      <c r="C47">
-        <v>554348</v>
-      </c>
-      <c r="D47">
-        <v>783326</v>
-      </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
@@ -2739,12 +2686,6 @@
       <c r="B48" t="s">
         <v>31</v>
       </c>
-      <c r="C48">
-        <v>372333</v>
-      </c>
-      <c r="D48">
-        <v>549858</v>
-      </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
@@ -2753,12 +2694,6 @@
       <c r="B49" t="s">
         <v>32</v>
       </c>
-      <c r="C49">
-        <v>125546</v>
-      </c>
-      <c r="D49">
-        <v>182968</v>
-      </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
@@ -2767,12 +2702,6 @@
       <c r="B50" t="s">
         <v>33</v>
       </c>
-      <c r="C50">
-        <v>55202</v>
-      </c>
-      <c r="D50">
-        <v>62458</v>
-      </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
@@ -2781,12 +2710,6 @@
       <c r="B51" t="s">
         <v>34</v>
       </c>
-      <c r="C51">
-        <v>171514</v>
-      </c>
-      <c r="D51">
-        <v>207128</v>
-      </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
@@ -2795,12 +2718,6 @@
       <c r="B52" t="s">
         <v>35</v>
       </c>
-      <c r="C52">
-        <v>91205</v>
-      </c>
-      <c r="D52">
-        <v>130476</v>
-      </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
@@ -2809,12 +2726,6 @@
       <c r="B53" t="s">
         <v>36</v>
       </c>
-      <c r="C53">
-        <v>58071</v>
-      </c>
-      <c r="D53">
-        <v>43211</v>
-      </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
@@ -2823,12 +2734,6 @@
       <c r="B54" t="s">
         <v>37</v>
       </c>
-      <c r="C54">
-        <v>56692</v>
-      </c>
-      <c r="D54">
-        <v>42110</v>
-      </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
@@ -2838,10 +2743,10 @@
         <v>38</v>
       </c>
       <c r="C55">
-        <v>33000</v>
+        <v>21441</v>
       </c>
       <c r="D55">
-        <v>21441</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
@@ -2852,10 +2757,10 @@
         <v>39</v>
       </c>
       <c r="C56">
-        <v>162272</v>
+        <v>126590</v>
       </c>
       <c r="D56">
-        <v>126590</v>
+        <v>24852</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
@@ -2866,10 +2771,10 @@
         <v>40</v>
       </c>
       <c r="C57">
-        <v>22621</v>
+        <v>15919</v>
       </c>
       <c r="D57">
-        <v>15919</v>
+        <v>3204</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
@@ -2880,10 +2785,10 @@
         <v>41</v>
       </c>
       <c r="C58">
-        <v>151905</v>
+        <v>103526</v>
       </c>
       <c r="D58">
-        <v>103526</v>
+        <v>17630</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
@@ -2894,10 +2799,10 @@
         <v>38</v>
       </c>
       <c r="C59">
-        <v>37939</v>
+        <v>24875</v>
       </c>
       <c r="D59">
-        <v>24875</v>
+        <v>1242</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
@@ -2908,10 +2813,10 @@
         <v>39</v>
       </c>
       <c r="C60">
-        <v>174900</v>
+        <v>138426</v>
       </c>
       <c r="D60">
-        <v>138426</v>
+        <v>29127</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
@@ -2922,10 +2827,10 @@
         <v>40</v>
       </c>
       <c r="C61">
-        <v>26041</v>
+        <v>20546</v>
       </c>
       <c r="D61">
-        <v>20546</v>
+        <v>5519</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
@@ -2936,10 +2841,10 @@
         <v>41</v>
       </c>
       <c r="C62">
-        <v>160068</v>
+        <v>111021</v>
       </c>
       <c r="D62">
-        <v>111021</v>
+        <v>18931</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
@@ -2950,10 +2855,10 @@
         <v>43</v>
       </c>
       <c r="C63">
-        <v>9068</v>
+        <v>11627</v>
       </c>
       <c r="D63">
-        <v>11627</v>
+        <v>8300</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
@@ -2963,39 +2868,21 @@
       <c r="B64" t="s">
         <v>42</v>
       </c>
-      <c r="C64">
-        <v>23488</v>
-      </c>
-      <c r="D64">
-        <v>23444</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>14</v>
       </c>
       <c r="B65" t="s">
         <v>42</v>
       </c>
-      <c r="C65">
-        <v>25502</v>
-      </c>
-      <c r="D65">
-        <v>26856</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>14</v>
       </c>
       <c r="B66" t="s">
         <v>44</v>
-      </c>
-      <c r="C66">
-        <v>9842</v>
-      </c>
-      <c r="D66">
-        <v>8957</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added in nativity data
</commit_message>
<xml_diff>
--- a/national_dta.xlsx
+++ b/national_dta.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-33600" yWindow="460" windowWidth="33600" windowHeight="20540" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="-33600" yWindow="460" windowWidth="33600" windowHeight="20540" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="edu" sheetId="5" r:id="rId1"/>
     <sheet name="cvap" sheetId="4" r:id="rId2"/>
     <sheet name="lep" sheetId="6" r:id="rId3"/>
+    <sheet name="nativity" sheetId="7" r:id="rId4"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="112">
   <si>
     <t>total_pop</t>
   </si>
@@ -344,13 +345,34 @@
   </si>
   <si>
     <t>checking_other_lang</t>
+  </si>
+  <si>
+    <t>est_tot_pop</t>
+  </si>
+  <si>
+    <t>moe_tot_pop</t>
+  </si>
+  <si>
+    <t>checking_tot_pop</t>
+  </si>
+  <si>
+    <t>est_foreign</t>
+  </si>
+  <si>
+    <t>moe_foreign</t>
+  </si>
+  <si>
+    <t>checking_foreign</t>
+  </si>
+  <si>
+    <t>pct_foreign</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -372,6 +394,11 @@
       <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -399,8 +426,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -5539,7 +5567,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -8503,4 +8531,2323 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J72"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P31" sqref="P31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1">
+        <v>316515008</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2" s="1">
+        <v>41717420</v>
+      </c>
+      <c r="H2" s="1">
+        <v>104288</v>
+      </c>
+      <c r="I2" s="1">
+        <v>0</v>
+      </c>
+      <c r="J2" s="1">
+        <v>0.13180235000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C3" s="1">
+        <v>4</v>
+      </c>
+      <c r="D3" s="1">
+        <v>39908096</v>
+      </c>
+      <c r="E3" s="1">
+        <v>26702</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1">
+        <v>3599684</v>
+      </c>
+      <c r="H3" s="1">
+        <v>21590</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0</v>
+      </c>
+      <c r="J3" s="1">
+        <v>9.0199344000000001E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" s="1">
+        <v>6</v>
+      </c>
+      <c r="D4" s="1">
+        <v>2569170</v>
+      </c>
+      <c r="E4" s="1">
+        <v>14914</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4" s="1">
+        <v>151490</v>
+      </c>
+      <c r="H4" s="1">
+        <v>4399</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0</v>
+      </c>
+      <c r="J4" s="1">
+        <v>5.8964569000000001E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" s="1">
+        <v>12</v>
+      </c>
+      <c r="D5" s="1">
+        <v>16235305</v>
+      </c>
+      <c r="E5" s="1">
+        <v>20725</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0</v>
+      </c>
+      <c r="G5" s="1">
+        <v>10796569</v>
+      </c>
+      <c r="H5" s="1">
+        <v>18202</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0.66500562399999996</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" s="1">
+        <v>13</v>
+      </c>
+      <c r="D6" s="1">
+        <v>3303512</v>
+      </c>
+      <c r="E6" s="1">
+        <v>17090</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1">
+        <v>2356160</v>
+      </c>
+      <c r="H6" s="1">
+        <v>12811</v>
+      </c>
+      <c r="I6" s="1">
+        <v>0</v>
+      </c>
+      <c r="J6" s="1">
+        <v>0.71322882200000004</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C7" s="1">
+        <v>14</v>
+      </c>
+      <c r="D7" s="1">
+        <v>153234</v>
+      </c>
+      <c r="E7" s="1">
+        <v>5479</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1">
+        <v>114126</v>
+      </c>
+      <c r="H7" s="1">
+        <v>4372</v>
+      </c>
+      <c r="I7" s="1">
+        <v>0</v>
+      </c>
+      <c r="J7" s="1">
+        <v>0.74478250700000004</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" s="1">
+        <v>15</v>
+      </c>
+      <c r="D8" s="1">
+        <v>263396</v>
+      </c>
+      <c r="E8" s="1">
+        <v>8409</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1">
+        <v>154178</v>
+      </c>
+      <c r="H8" s="1">
+        <v>5035</v>
+      </c>
+      <c r="I8" s="1">
+        <v>0</v>
+      </c>
+      <c r="J8" s="1">
+        <v>0.58534675800000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C9" s="1">
+        <v>16</v>
+      </c>
+      <c r="D9" s="1">
+        <v>3852099</v>
+      </c>
+      <c r="E9" s="1">
+        <v>19831</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1">
+        <v>2672930</v>
+      </c>
+      <c r="H9" s="1">
+        <v>13916</v>
+      </c>
+      <c r="I9" s="1">
+        <v>0</v>
+      </c>
+      <c r="J9" s="1">
+        <v>0.69388920099999996</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C10" s="1">
+        <v>17</v>
+      </c>
+      <c r="D10" s="1">
+        <v>3693977</v>
+      </c>
+      <c r="E10" s="1">
+        <v>18855</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1">
+        <v>2560943</v>
+      </c>
+      <c r="H10" s="1">
+        <v>13675</v>
+      </c>
+      <c r="I10" s="1">
+        <v>0</v>
+      </c>
+      <c r="J10" s="1">
+        <v>0.69327527300000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C11" s="1">
+        <v>18</v>
+      </c>
+      <c r="D11" s="1">
+        <v>148275</v>
+      </c>
+      <c r="E11" s="1">
+        <v>4247</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0</v>
+      </c>
+      <c r="G11" s="1">
+        <v>105500</v>
+      </c>
+      <c r="H11" s="1">
+        <v>3198</v>
+      </c>
+      <c r="I11" s="1">
+        <v>0</v>
+      </c>
+      <c r="J11" s="1">
+        <v>0.71151578400000004</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C12" s="1">
+        <v>19</v>
+      </c>
+      <c r="D12" s="1">
+        <v>2717844</v>
+      </c>
+      <c r="E12" s="1">
+        <v>17934</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0</v>
+      </c>
+      <c r="G12" s="1">
+        <v>1787850</v>
+      </c>
+      <c r="H12" s="1">
+        <v>13581</v>
+      </c>
+      <c r="I12" s="1">
+        <v>0</v>
+      </c>
+      <c r="J12" s="1">
+        <v>0.65781921099999996</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C13" s="1">
+        <v>20</v>
+      </c>
+      <c r="D13" s="1">
+        <v>267009</v>
+      </c>
+      <c r="E13" s="1">
+        <v>6734</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0</v>
+      </c>
+      <c r="G13" s="1">
+        <v>104775</v>
+      </c>
+      <c r="H13" s="1">
+        <v>3093</v>
+      </c>
+      <c r="I13" s="1">
+        <v>0</v>
+      </c>
+      <c r="J13" s="1">
+        <v>0.39240249999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C14" s="1">
+        <v>21</v>
+      </c>
+      <c r="D14" s="1">
+        <v>71451</v>
+      </c>
+      <c r="E14" s="1">
+        <v>2920</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0</v>
+      </c>
+      <c r="G14" s="1">
+        <v>55213</v>
+      </c>
+      <c r="H14" s="1">
+        <v>2261</v>
+      </c>
+      <c r="I14" s="1">
+        <v>0</v>
+      </c>
+      <c r="J14" s="1">
+        <v>0.77273935100000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C15" s="1">
+        <v>22</v>
+      </c>
+      <c r="D15" s="1">
+        <v>779637</v>
+      </c>
+      <c r="E15" s="1">
+        <v>9694</v>
+      </c>
+      <c r="F15" s="1">
+        <v>0</v>
+      </c>
+      <c r="G15" s="1">
+        <v>313689</v>
+      </c>
+      <c r="H15" s="1">
+        <v>5833</v>
+      </c>
+      <c r="I15" s="1">
+        <v>0</v>
+      </c>
+      <c r="J15" s="1">
+        <v>0.40235263100000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C16" s="1">
+        <v>23</v>
+      </c>
+      <c r="D16" s="1">
+        <v>1460214</v>
+      </c>
+      <c r="E16" s="1">
+        <v>13339</v>
+      </c>
+      <c r="F16" s="1">
+        <v>0</v>
+      </c>
+      <c r="G16" s="1">
+        <v>1062693</v>
+      </c>
+      <c r="H16" s="1">
+        <v>10158</v>
+      </c>
+      <c r="I16" s="1">
+        <v>0</v>
+      </c>
+      <c r="J16" s="1">
+        <v>0.72776526200000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C17" s="1">
+        <v>24</v>
+      </c>
+      <c r="D17" s="1">
+        <v>207999</v>
+      </c>
+      <c r="E17" s="1">
+        <v>4997</v>
+      </c>
+      <c r="F17" s="1">
+        <v>0</v>
+      </c>
+      <c r="G17" s="1">
+        <v>120363</v>
+      </c>
+      <c r="H17" s="1">
+        <v>3053</v>
+      </c>
+      <c r="I17" s="1">
+        <v>0</v>
+      </c>
+      <c r="J17" s="1">
+        <v>0.57867103799999997</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C18" s="1">
+        <v>25</v>
+      </c>
+      <c r="D18" s="1">
+        <v>18803</v>
+      </c>
+      <c r="E18" s="1">
+        <v>1544</v>
+      </c>
+      <c r="F18" s="1">
+        <v>0</v>
+      </c>
+      <c r="G18" s="1">
+        <v>15706</v>
+      </c>
+      <c r="H18" s="1">
+        <v>1292</v>
+      </c>
+      <c r="I18" s="1">
+        <v>0</v>
+      </c>
+      <c r="J18" s="1">
+        <v>0.83529222000000003</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C19" s="1">
+        <v>26</v>
+      </c>
+      <c r="D19" s="1">
+        <v>414880</v>
+      </c>
+      <c r="E19" s="1">
+        <v>11430</v>
+      </c>
+      <c r="F19" s="1">
+        <v>0</v>
+      </c>
+      <c r="G19" s="1">
+        <v>274990</v>
+      </c>
+      <c r="H19" s="1">
+        <v>7509</v>
+      </c>
+      <c r="I19" s="1">
+        <v>0</v>
+      </c>
+      <c r="J19" s="1">
+        <v>0.662818193</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C20" s="1">
+        <v>27</v>
+      </c>
+      <c r="D20" s="1">
+        <v>46036</v>
+      </c>
+      <c r="E20" s="1">
+        <v>2724</v>
+      </c>
+      <c r="F20" s="1">
+        <v>0</v>
+      </c>
+      <c r="G20" s="1">
+        <v>35733</v>
+      </c>
+      <c r="H20" s="1">
+        <v>2214</v>
+      </c>
+      <c r="I20" s="1">
+        <v>0</v>
+      </c>
+      <c r="J20" s="1">
+        <v>0.77619689700000005</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C21" s="1">
+        <v>28</v>
+      </c>
+      <c r="D21" s="1">
+        <v>188673</v>
+      </c>
+      <c r="E21" s="1">
+        <v>4784</v>
+      </c>
+      <c r="F21" s="1">
+        <v>0</v>
+      </c>
+      <c r="G21" s="1">
+        <v>142997</v>
+      </c>
+      <c r="H21" s="1">
+        <v>3875</v>
+      </c>
+      <c r="I21" s="1">
+        <v>0</v>
+      </c>
+      <c r="J21" s="1">
+        <v>0.75790917899999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C22" s="1">
+        <v>29</v>
+      </c>
+      <c r="D22" s="1">
+        <v>1710547</v>
+      </c>
+      <c r="E22" s="1">
+        <v>18780</v>
+      </c>
+      <c r="F22" s="1">
+        <v>0</v>
+      </c>
+      <c r="G22" s="1">
+        <v>1155190</v>
+      </c>
+      <c r="H22" s="1">
+        <v>12122</v>
+      </c>
+      <c r="I22" s="1">
+        <v>0</v>
+      </c>
+      <c r="J22" s="1">
+        <v>0.67533367899999996</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C23" s="1">
+        <v>31</v>
+      </c>
+      <c r="D23" s="1">
+        <v>19167716</v>
+      </c>
+      <c r="E23" s="1">
+        <v>19485</v>
+      </c>
+      <c r="F23" s="1">
+        <v>0</v>
+      </c>
+      <c r="G23" s="1">
+        <v>11255240</v>
+      </c>
+      <c r="H23" s="1">
+        <v>17891</v>
+      </c>
+      <c r="I23" s="1">
+        <v>0</v>
+      </c>
+      <c r="J23" s="1">
+        <v>0.58719778099999997</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C24" s="1">
+        <v>32</v>
+      </c>
+      <c r="D24" s="1">
+        <v>3590279</v>
+      </c>
+      <c r="E24" s="1">
+        <v>16777</v>
+      </c>
+      <c r="F24" s="1">
+        <v>0</v>
+      </c>
+      <c r="G24" s="1">
+        <v>2452196</v>
+      </c>
+      <c r="H24" s="1">
+        <v>13073</v>
+      </c>
+      <c r="I24" s="1">
+        <v>0</v>
+      </c>
+      <c r="J24" s="1">
+        <v>0.68300986299999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C25" s="1">
+        <v>33</v>
+      </c>
+      <c r="D25" s="1">
+        <v>164821</v>
+      </c>
+      <c r="E25" s="1">
+        <v>5618</v>
+      </c>
+      <c r="F25" s="1">
+        <v>0</v>
+      </c>
+      <c r="G25" s="1">
+        <v>120769</v>
+      </c>
+      <c r="H25" s="1">
+        <v>4439</v>
+      </c>
+      <c r="I25" s="1">
+        <v>0</v>
+      </c>
+      <c r="J25" s="1">
+        <v>0.73272824299999995</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C26" s="1">
+        <v>34</v>
+      </c>
+      <c r="D26" s="1">
+        <v>316640</v>
+      </c>
+      <c r="E26" s="1">
+        <v>8596</v>
+      </c>
+      <c r="F26" s="1">
+        <v>0</v>
+      </c>
+      <c r="G26" s="1">
+        <v>166018</v>
+      </c>
+      <c r="H26" s="1">
+        <v>4976</v>
+      </c>
+      <c r="I26" s="1">
+        <v>0</v>
+      </c>
+      <c r="J26" s="1">
+        <v>0.52431154300000005</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C27" s="1">
+        <v>35</v>
+      </c>
+      <c r="D27" s="1">
+        <v>4597905</v>
+      </c>
+      <c r="E27" s="1">
+        <v>24921</v>
+      </c>
+      <c r="F27" s="1">
+        <v>0</v>
+      </c>
+      <c r="G27" s="1">
+        <v>2787690</v>
+      </c>
+      <c r="H27" s="1">
+        <v>14728</v>
+      </c>
+      <c r="I27" s="1">
+        <v>0</v>
+      </c>
+      <c r="J27" s="1">
+        <v>0.60629570499999996</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C28" s="1">
+        <v>36</v>
+      </c>
+      <c r="D28" s="1">
+        <v>4428363</v>
+      </c>
+      <c r="E28" s="1">
+        <v>23401</v>
+      </c>
+      <c r="F28" s="1">
+        <v>0</v>
+      </c>
+      <c r="G28" s="1">
+        <v>2678781</v>
+      </c>
+      <c r="H28" s="1">
+        <v>14464</v>
+      </c>
+      <c r="I28" s="1">
+        <v>0</v>
+      </c>
+      <c r="J28" s="1">
+        <v>0.60491448599999997</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C29" s="1">
+        <v>37</v>
+      </c>
+      <c r="D29" s="1">
+        <v>181029</v>
+      </c>
+      <c r="E29" s="1">
+        <v>4898</v>
+      </c>
+      <c r="F29" s="1">
+        <v>0</v>
+      </c>
+      <c r="G29" s="1">
+        <v>115720</v>
+      </c>
+      <c r="H29" s="1">
+        <v>3328</v>
+      </c>
+      <c r="I29" s="1">
+        <v>0</v>
+      </c>
+      <c r="J29" s="1">
+        <v>0.63923460200000004</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C30" s="1">
+        <v>38</v>
+      </c>
+      <c r="D30" s="1">
+        <v>3707082</v>
+      </c>
+      <c r="E30" s="1">
+        <v>24374</v>
+      </c>
+      <c r="F30" s="1">
+        <v>0</v>
+      </c>
+      <c r="G30" s="1">
+        <v>1875044</v>
+      </c>
+      <c r="H30" s="1">
+        <v>13593</v>
+      </c>
+      <c r="I30" s="1">
+        <v>0</v>
+      </c>
+      <c r="J30" s="1">
+        <v>0.50580054500000005</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C31" s="1">
+        <v>39</v>
+      </c>
+      <c r="D31" s="1">
+        <v>280410</v>
+      </c>
+      <c r="E31" s="1">
+        <v>6971</v>
+      </c>
+      <c r="F31" s="1">
+        <v>0</v>
+      </c>
+      <c r="G31" s="1">
+        <v>107630</v>
+      </c>
+      <c r="H31" s="1">
+        <v>3267</v>
+      </c>
+      <c r="I31" s="1">
+        <v>0</v>
+      </c>
+      <c r="J31" s="1">
+        <v>0.38383081600000002</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C32" s="1">
+        <v>40</v>
+      </c>
+      <c r="D32" s="1">
+        <v>108477</v>
+      </c>
+      <c r="E32" s="1">
+        <v>3749</v>
+      </c>
+      <c r="F32" s="1">
+        <v>0</v>
+      </c>
+      <c r="G32" s="1">
+        <v>66041</v>
+      </c>
+      <c r="H32" s="1">
+        <v>2498</v>
+      </c>
+      <c r="I32" s="1">
+        <v>0</v>
+      </c>
+      <c r="J32" s="1">
+        <v>0.60880184199999998</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C33" s="1">
+        <v>41</v>
+      </c>
+      <c r="D33" s="1">
+        <v>1388163</v>
+      </c>
+      <c r="E33" s="1">
+        <v>15805</v>
+      </c>
+      <c r="F33" s="1">
+        <v>0</v>
+      </c>
+      <c r="G33" s="1">
+        <v>341479</v>
+      </c>
+      <c r="H33" s="1">
+        <v>6224</v>
+      </c>
+      <c r="I33" s="1">
+        <v>0</v>
+      </c>
+      <c r="J33" s="1">
+        <v>0.24599345</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C34" s="1">
+        <v>42</v>
+      </c>
+      <c r="D34" s="1">
+        <v>1792437</v>
+      </c>
+      <c r="E34" s="1">
+        <v>14297</v>
+      </c>
+      <c r="F34" s="1">
+        <v>0</v>
+      </c>
+      <c r="G34" s="1">
+        <v>1081982</v>
+      </c>
+      <c r="H34" s="1">
+        <v>10187</v>
+      </c>
+      <c r="I34" s="1">
+        <v>0</v>
+      </c>
+      <c r="J34" s="1">
+        <v>0.60363739699999996</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C35" s="1">
+        <v>43</v>
+      </c>
+      <c r="D35" s="1">
+        <v>256416</v>
+      </c>
+      <c r="E35" s="1">
+        <v>5432</v>
+      </c>
+      <c r="F35" s="1">
+        <v>0</v>
+      </c>
+      <c r="G35" s="1">
+        <v>126666</v>
+      </c>
+      <c r="H35" s="1">
+        <v>3210</v>
+      </c>
+      <c r="I35" s="1">
+        <v>0</v>
+      </c>
+      <c r="J35" s="1">
+        <v>0.49398633800000002</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C36" s="1">
+        <v>44</v>
+      </c>
+      <c r="D36" s="1">
+        <v>28818</v>
+      </c>
+      <c r="E36" s="1">
+        <v>1890</v>
+      </c>
+      <c r="F36" s="1">
+        <v>0</v>
+      </c>
+      <c r="G36" s="1">
+        <v>20332</v>
+      </c>
+      <c r="H36" s="1">
+        <v>1461</v>
+      </c>
+      <c r="I36" s="1">
+        <v>0</v>
+      </c>
+      <c r="J36" s="1">
+        <v>0.70553124</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C37" s="1">
+        <v>45</v>
+      </c>
+      <c r="D37" s="1">
+        <v>455005</v>
+      </c>
+      <c r="E37" s="1">
+        <v>11349</v>
+      </c>
+      <c r="F37" s="1">
+        <v>0</v>
+      </c>
+      <c r="G37" s="1">
+        <v>287193</v>
+      </c>
+      <c r="H37" s="1">
+        <v>7562</v>
+      </c>
+      <c r="I37" s="1">
+        <v>0</v>
+      </c>
+      <c r="J37" s="1">
+        <v>0.63118648499999996</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C38" s="1">
+        <v>46</v>
+      </c>
+      <c r="D38" s="1">
+        <v>52267</v>
+      </c>
+      <c r="E38" s="1">
+        <v>2925</v>
+      </c>
+      <c r="F38" s="1">
+        <v>0</v>
+      </c>
+      <c r="G38" s="1">
+        <v>37855</v>
+      </c>
+      <c r="H38" s="1">
+        <v>2324</v>
+      </c>
+      <c r="I38" s="1">
+        <v>0</v>
+      </c>
+      <c r="J38" s="1">
+        <v>0.72426193999999999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C39" s="1">
+        <v>47</v>
+      </c>
+      <c r="D39" s="1">
+        <v>278281</v>
+      </c>
+      <c r="E39" s="1">
+        <v>5520</v>
+      </c>
+      <c r="F39" s="1">
+        <v>0</v>
+      </c>
+      <c r="G39" s="1">
+        <v>153140</v>
+      </c>
+      <c r="H39" s="1">
+        <v>3723</v>
+      </c>
+      <c r="I39" s="1">
+        <v>0</v>
+      </c>
+      <c r="J39" s="1">
+        <v>0.550307035</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C40" s="1">
+        <v>48</v>
+      </c>
+      <c r="D40" s="1">
+        <v>1928363</v>
+      </c>
+      <c r="E40" s="1">
+        <v>19234</v>
+      </c>
+      <c r="F40" s="1">
+        <v>0</v>
+      </c>
+      <c r="G40" s="1">
+        <v>1204976</v>
+      </c>
+      <c r="H40" s="1">
+        <v>12576</v>
+      </c>
+      <c r="I40" s="1">
+        <v>0</v>
+      </c>
+      <c r="J40" s="1">
+        <v>0.62486988300000001</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C41" s="1">
+        <v>50</v>
+      </c>
+      <c r="D41" s="1">
+        <v>546255</v>
+      </c>
+      <c r="E41" s="1">
+        <v>4552</v>
+      </c>
+      <c r="F41" s="1">
+        <v>0</v>
+      </c>
+      <c r="G41" s="1">
+        <v>115677</v>
+      </c>
+      <c r="H41" s="1">
+        <v>3289</v>
+      </c>
+      <c r="I41" s="1">
+        <v>0</v>
+      </c>
+      <c r="J41" s="1">
+        <v>0.21176374000000001</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C42" s="1">
+        <v>51</v>
+      </c>
+      <c r="D42" s="1">
+        <v>344487</v>
+      </c>
+      <c r="E42" s="1">
+        <v>4839</v>
+      </c>
+      <c r="F42" s="1">
+        <v>0</v>
+      </c>
+      <c r="G42" s="1">
+        <v>38547</v>
+      </c>
+      <c r="H42" s="1">
+        <v>1693</v>
+      </c>
+      <c r="I42" s="1">
+        <v>0</v>
+      </c>
+      <c r="J42" s="1">
+        <v>0.11189681999999999</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C43" s="1">
+        <v>52</v>
+      </c>
+      <c r="D43" s="1">
+        <v>174460</v>
+      </c>
+      <c r="E43" s="1">
+        <v>4519</v>
+      </c>
+      <c r="F43" s="1">
+        <v>0</v>
+      </c>
+      <c r="G43" s="1">
+        <v>4167</v>
+      </c>
+      <c r="H43" s="1">
+        <v>646</v>
+      </c>
+      <c r="I43" s="1">
+        <v>0</v>
+      </c>
+      <c r="J43" s="1">
+        <v>2.3885131E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C44" s="1">
+        <v>53</v>
+      </c>
+      <c r="D44" s="1">
+        <v>109455</v>
+      </c>
+      <c r="E44" s="1">
+        <v>3835</v>
+      </c>
+      <c r="F44" s="1">
+        <v>0</v>
+      </c>
+      <c r="G44" s="1">
+        <v>13274</v>
+      </c>
+      <c r="H44" s="1">
+        <v>977</v>
+      </c>
+      <c r="I44" s="1">
+        <v>0</v>
+      </c>
+      <c r="J44" s="1">
+        <v>0.121273585</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C45" s="1">
+        <v>54</v>
+      </c>
+      <c r="D45" s="1">
+        <v>45453</v>
+      </c>
+      <c r="E45" s="1">
+        <v>2981</v>
+      </c>
+      <c r="F45" s="1">
+        <v>0</v>
+      </c>
+      <c r="G45" s="1">
+        <v>18652</v>
+      </c>
+      <c r="H45" s="1">
+        <v>1358</v>
+      </c>
+      <c r="I45" s="1">
+        <v>0</v>
+      </c>
+      <c r="J45" s="1">
+        <v>0.41035795200000003</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C46" s="1">
+        <v>55</v>
+      </c>
+      <c r="D46" s="1">
+        <v>138360</v>
+      </c>
+      <c r="E46" s="1">
+        <v>3689</v>
+      </c>
+      <c r="F46" s="1">
+        <v>0</v>
+      </c>
+      <c r="G46" s="1">
+        <v>44931</v>
+      </c>
+      <c r="H46" s="1">
+        <v>2309</v>
+      </c>
+      <c r="I46" s="1">
+        <v>0</v>
+      </c>
+      <c r="J46" s="1">
+        <v>0.32473981400000002</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C47" s="1">
+        <v>56</v>
+      </c>
+      <c r="D47" s="1">
+        <v>73088</v>
+      </c>
+      <c r="E47" s="1">
+        <v>2797</v>
+      </c>
+      <c r="F47" s="1">
+        <v>0</v>
+      </c>
+      <c r="G47" s="1">
+        <v>4874</v>
+      </c>
+      <c r="H47" s="1">
+        <v>674</v>
+      </c>
+      <c r="I47" s="1">
+        <v>0</v>
+      </c>
+      <c r="J47" s="1">
+        <v>6.6686734999999997E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C48" s="1">
+        <v>57</v>
+      </c>
+      <c r="D48" s="1">
+        <v>34239</v>
+      </c>
+      <c r="E48" s="1">
+        <v>1993</v>
+      </c>
+      <c r="F48" s="1">
+        <v>0</v>
+      </c>
+      <c r="G48" s="1">
+        <v>23816</v>
+      </c>
+      <c r="H48" s="1">
+        <v>1436</v>
+      </c>
+      <c r="I48" s="1">
+        <v>0</v>
+      </c>
+      <c r="J48" s="1">
+        <v>0.69558107899999999</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C49" s="1">
+        <v>58</v>
+      </c>
+      <c r="D49" s="1">
+        <v>33468</v>
+      </c>
+      <c r="E49" s="1">
+        <v>1972</v>
+      </c>
+      <c r="F49" s="1">
+        <v>0</v>
+      </c>
+      <c r="G49" s="1">
+        <v>23221</v>
+      </c>
+      <c r="H49" s="1">
+        <v>1416</v>
+      </c>
+      <c r="I49" s="1">
+        <v>0</v>
+      </c>
+      <c r="J49" s="1">
+        <v>0.69382691399999996</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C50" s="1">
+        <v>60</v>
+      </c>
+      <c r="D50" s="1">
+        <v>1262434</v>
+      </c>
+      <c r="E50" s="1">
+        <v>9700</v>
+      </c>
+      <c r="F50" s="1">
+        <v>0</v>
+      </c>
+      <c r="G50" s="1">
+        <v>208855</v>
+      </c>
+      <c r="H50" s="1">
+        <v>4566</v>
+      </c>
+      <c r="I50" s="1">
+        <v>0</v>
+      </c>
+      <c r="J50" s="1">
+        <v>0.16543835400000001</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C51" s="1">
+        <v>61</v>
+      </c>
+      <c r="D51" s="1">
+        <v>783326</v>
+      </c>
+      <c r="E51" s="1">
+        <v>7279</v>
+      </c>
+      <c r="F51" s="1">
+        <v>0</v>
+      </c>
+      <c r="G51" s="1">
+        <v>46988</v>
+      </c>
+      <c r="H51" s="1">
+        <v>1852</v>
+      </c>
+      <c r="I51" s="1">
+        <v>0</v>
+      </c>
+      <c r="J51" s="1">
+        <v>5.9985243000000001E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C52" s="1">
+        <v>62</v>
+      </c>
+      <c r="D52" s="1">
+        <v>549858</v>
+      </c>
+      <c r="E52" s="1">
+        <v>8077</v>
+      </c>
+      <c r="F52" s="1">
+        <v>0</v>
+      </c>
+      <c r="G52" s="1">
+        <v>8625</v>
+      </c>
+      <c r="H52" s="1">
+        <v>840</v>
+      </c>
+      <c r="I52" s="1">
+        <v>0</v>
+      </c>
+      <c r="J52" s="1">
+        <v>1.5685867999999999E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C53" s="1">
+        <v>63</v>
+      </c>
+      <c r="D53" s="1">
+        <v>182968</v>
+      </c>
+      <c r="E53" s="1">
+        <v>5079</v>
+      </c>
+      <c r="F53" s="1">
+        <v>0</v>
+      </c>
+      <c r="G53" s="1">
+        <v>15568</v>
+      </c>
+      <c r="H53" s="1">
+        <v>1091</v>
+      </c>
+      <c r="I53" s="1">
+        <v>0</v>
+      </c>
+      <c r="J53" s="1">
+        <v>8.5085913999999999E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C54" s="1">
+        <v>64</v>
+      </c>
+      <c r="D54" s="1">
+        <v>62458</v>
+      </c>
+      <c r="E54" s="1">
+        <v>3119</v>
+      </c>
+      <c r="F54" s="1">
+        <v>0</v>
+      </c>
+      <c r="G54" s="1">
+        <v>19716</v>
+      </c>
+      <c r="H54" s="1">
+        <v>1318</v>
+      </c>
+      <c r="I54" s="1">
+        <v>0</v>
+      </c>
+      <c r="J54" s="1">
+        <v>0.31566813599999999</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A55" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C55" s="1">
+        <v>65</v>
+      </c>
+      <c r="D55" s="1">
+        <v>207128</v>
+      </c>
+      <c r="E55" s="1">
+        <v>4178</v>
+      </c>
+      <c r="F55" s="1">
+        <v>0</v>
+      </c>
+      <c r="G55" s="1">
+        <v>49264</v>
+      </c>
+      <c r="H55" s="1">
+        <v>2324</v>
+      </c>
+      <c r="I55" s="1">
+        <v>0</v>
+      </c>
+      <c r="J55" s="1">
+        <v>0.23784326</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C56" s="1">
+        <v>66</v>
+      </c>
+      <c r="D56" s="1">
+        <v>130476</v>
+      </c>
+      <c r="E56" s="1">
+        <v>3970</v>
+      </c>
+      <c r="F56" s="1">
+        <v>0</v>
+      </c>
+      <c r="G56" s="1">
+        <v>6944</v>
+      </c>
+      <c r="H56" s="1">
+        <v>795</v>
+      </c>
+      <c r="I56" s="1">
+        <v>0</v>
+      </c>
+      <c r="J56" s="1">
+        <v>5.3220513999999997E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A57" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C57" s="1">
+        <v>67</v>
+      </c>
+      <c r="D57" s="1">
+        <v>43211</v>
+      </c>
+      <c r="E57" s="1">
+        <v>2222</v>
+      </c>
+      <c r="F57" s="1">
+        <v>0</v>
+      </c>
+      <c r="G57" s="1">
+        <v>27260</v>
+      </c>
+      <c r="H57" s="1">
+        <v>1575</v>
+      </c>
+      <c r="I57" s="1">
+        <v>0</v>
+      </c>
+      <c r="J57" s="1">
+        <v>0.63085788499999995</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A58" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C58" s="1">
+        <v>68</v>
+      </c>
+      <c r="D58" s="1">
+        <v>42110</v>
+      </c>
+      <c r="E58" s="1">
+        <v>2220</v>
+      </c>
+      <c r="F58" s="1">
+        <v>0</v>
+      </c>
+      <c r="G58" s="1">
+        <v>26564</v>
+      </c>
+      <c r="H58" s="1">
+        <v>1559</v>
+      </c>
+      <c r="I58" s="1">
+        <v>0</v>
+      </c>
+      <c r="J58" s="1">
+        <v>0.63082402900000001</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A59" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C59" s="1">
+        <v>72</v>
+      </c>
+      <c r="D59" s="1">
+        <v>21441</v>
+      </c>
+      <c r="E59" s="1">
+        <v>2416</v>
+      </c>
+      <c r="F59" s="1">
+        <v>0</v>
+      </c>
+      <c r="G59" s="1">
+        <v>19542</v>
+      </c>
+      <c r="H59" s="1">
+        <v>2234</v>
+      </c>
+      <c r="I59" s="1">
+        <v>0</v>
+      </c>
+      <c r="J59" s="1">
+        <v>0.91143137200000002</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A60" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C60" s="1">
+        <v>73</v>
+      </c>
+      <c r="D60" s="1">
+        <v>126590</v>
+      </c>
+      <c r="E60" s="1">
+        <v>5388</v>
+      </c>
+      <c r="F60" s="1">
+        <v>0</v>
+      </c>
+      <c r="G60" s="1">
+        <v>108502</v>
+      </c>
+      <c r="H60" s="1">
+        <v>4691</v>
+      </c>
+      <c r="I60" s="1">
+        <v>0</v>
+      </c>
+      <c r="J60" s="1">
+        <v>0.85711353999999995</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A61" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C61" s="1">
+        <v>75</v>
+      </c>
+      <c r="D61" s="1">
+        <v>15919</v>
+      </c>
+      <c r="E61" s="1">
+        <v>1626</v>
+      </c>
+      <c r="F61" s="1">
+        <v>0</v>
+      </c>
+      <c r="G61" s="1">
+        <v>12276</v>
+      </c>
+      <c r="H61" s="1">
+        <v>1286</v>
+      </c>
+      <c r="I61" s="1">
+        <v>0</v>
+      </c>
+      <c r="J61" s="1">
+        <v>0.77115398599999996</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A62" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C62" s="1">
+        <v>76</v>
+      </c>
+      <c r="D62" s="1">
+        <v>103526</v>
+      </c>
+      <c r="E62" s="1">
+        <v>4285</v>
+      </c>
+      <c r="F62" s="1">
+        <v>0</v>
+      </c>
+      <c r="G62" s="1">
+        <v>90632</v>
+      </c>
+      <c r="H62" s="1">
+        <v>3786</v>
+      </c>
+      <c r="I62" s="1">
+        <v>0</v>
+      </c>
+      <c r="J62" s="1">
+        <v>0.87545156499999999</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A63" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C63" s="1">
+        <v>80</v>
+      </c>
+      <c r="D63" s="1">
+        <v>24875</v>
+      </c>
+      <c r="E63" s="1">
+        <v>2425</v>
+      </c>
+      <c r="F63" s="1">
+        <v>0</v>
+      </c>
+      <c r="G63" s="1">
+        <v>22723</v>
+      </c>
+      <c r="H63" s="1">
+        <v>2240</v>
+      </c>
+      <c r="I63" s="1">
+        <v>0</v>
+      </c>
+      <c r="J63" s="1">
+        <v>0.91348743399999999</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A64" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C64" s="1">
+        <v>81</v>
+      </c>
+      <c r="D64" s="1">
+        <v>138426</v>
+      </c>
+      <c r="E64" s="1">
+        <v>5576</v>
+      </c>
+      <c r="F64" s="1">
+        <v>0</v>
+      </c>
+      <c r="G64" s="1">
+        <v>115299</v>
+      </c>
+      <c r="H64" s="1">
+        <v>4773</v>
+      </c>
+      <c r="I64" s="1">
+        <v>0</v>
+      </c>
+      <c r="J64" s="1">
+        <v>0.83292877700000001</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A65" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C65" s="1">
+        <v>83</v>
+      </c>
+      <c r="D65" s="1">
+        <v>20546</v>
+      </c>
+      <c r="E65" s="1">
+        <v>1898</v>
+      </c>
+      <c r="F65" s="1">
+        <v>0</v>
+      </c>
+      <c r="G65" s="1">
+        <v>13121</v>
+      </c>
+      <c r="H65" s="1">
+        <v>1324</v>
+      </c>
+      <c r="I65" s="1">
+        <v>0</v>
+      </c>
+      <c r="J65" s="1">
+        <v>0.63861578699999999</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A66" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C66" s="1">
+        <v>84</v>
+      </c>
+      <c r="D66" s="1">
+        <v>111021</v>
+      </c>
+      <c r="E66" s="1">
+        <v>4578</v>
+      </c>
+      <c r="F66" s="1">
+        <v>0</v>
+      </c>
+      <c r="G66" s="1">
+        <v>95468</v>
+      </c>
+      <c r="H66" s="1">
+        <v>4002</v>
+      </c>
+      <c r="I66" s="1">
+        <v>0</v>
+      </c>
+      <c r="J66" s="1">
+        <v>0.85990941499999995</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A67" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C67" s="1">
+        <v>85</v>
+      </c>
+      <c r="D67" s="1">
+        <v>11627</v>
+      </c>
+      <c r="E67" s="1">
+        <v>870</v>
+      </c>
+      <c r="F67" s="1">
+        <v>0</v>
+      </c>
+      <c r="G67" s="1">
+        <v>593</v>
+      </c>
+      <c r="H67" s="1">
+        <v>146</v>
+      </c>
+      <c r="I67" s="1">
+        <v>0</v>
+      </c>
+      <c r="J67" s="1">
+        <v>5.1001976999999997E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A68" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C68" s="1">
+        <v>96</v>
+      </c>
+      <c r="D68" s="1">
+        <v>23444</v>
+      </c>
+      <c r="E68" s="1">
+        <v>1988</v>
+      </c>
+      <c r="F68" s="1">
+        <v>0</v>
+      </c>
+      <c r="G68" s="1">
+        <v>14489</v>
+      </c>
+      <c r="H68" s="1">
+        <v>1446</v>
+      </c>
+      <c r="I68" s="1">
+        <v>0</v>
+      </c>
+      <c r="J68" s="1">
+        <v>0.61802595900000001</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A69" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C69" s="1">
+        <v>176</v>
+      </c>
+      <c r="D69" s="1">
+        <v>26856</v>
+      </c>
+      <c r="E69" s="1">
+        <v>2368</v>
+      </c>
+      <c r="F69" s="1">
+        <v>0</v>
+      </c>
+      <c r="G69" s="1">
+        <v>15616</v>
+      </c>
+      <c r="H69" s="1">
+        <v>1601</v>
+      </c>
+      <c r="I69" s="1">
+        <v>0</v>
+      </c>
+      <c r="J69" s="1">
+        <v>0.58147156200000005</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A70" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C70" s="1">
+        <v>177</v>
+      </c>
+      <c r="D70" s="1">
+        <v>8957</v>
+      </c>
+      <c r="E70" s="1">
+        <v>1133</v>
+      </c>
+      <c r="F70" s="1">
+        <v>0</v>
+      </c>
+      <c r="G70" s="1">
+        <v>4054</v>
+      </c>
+      <c r="H70" s="1">
+        <v>657</v>
+      </c>
+      <c r="I70" s="1">
+        <v>0</v>
+      </c>
+      <c r="J70" s="1">
+        <v>0.45260688700000001</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A71" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C71" s="1">
+        <v>400</v>
+      </c>
+      <c r="D71" s="1">
+        <v>54232204</v>
+      </c>
+      <c r="E71" s="1">
+        <v>2036</v>
+      </c>
+      <c r="F71" s="1">
+        <v>0</v>
+      </c>
+      <c r="G71" s="1">
+        <v>19106796</v>
+      </c>
+      <c r="H71" s="1">
+        <v>60551</v>
+      </c>
+      <c r="I71" s="1">
+        <v>0</v>
+      </c>
+      <c r="J71" s="1">
+        <v>0.35231459100000001</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A72" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C72" s="1">
+        <v>451</v>
+      </c>
+      <c r="D72" s="1">
+        <v>197258272</v>
+      </c>
+      <c r="E72" s="1">
+        <v>8320</v>
+      </c>
+      <c r="F72" s="1">
+        <v>0</v>
+      </c>
+      <c r="G72" s="1">
+        <v>7646466</v>
+      </c>
+      <c r="H72" s="1">
+        <v>31450</v>
+      </c>
+      <c r="I72" s="1">
+        <v>0</v>
+      </c>
+      <c r="J72" s="1">
+        <v>3.8763727999999997E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>